<commit_message>
adding more specification files
</commit_message>
<xml_diff>
--- a/src/test_data/services_2.xlsx
+++ b/src/test_data/services_2.xlsx
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
   <si>
-    <t>patient_id</t>
-  </si>
-  <si>
     <t>service_id</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>P10</t>
+  </si>
+  <si>
+    <t>subject_id</t>
   </si>
 </sst>
 </file>
@@ -595,7 +595,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -608,255 +608,255 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>